<commit_message>
Updated figure names and added supplementary figure 4 of PDPs for dispersal and island dwelling. Added read me files to tables of binary predicitons.
</commit_message>
<xml_diff>
--- a/figures/other/hosttrait/table_binarypredictions_pcr.xlsx
+++ b/figures/other/hosttrait/table_binarypredictions_pcr.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/katie_tseng_wsu_edu/Documents/Fernandez Lab/Projects (Active)/OPV Host Prediction/GitHub/PoxHost/figures/other/hosttrait/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3A09A587BADDE2F2EEC00F81A82FAC824A35A5A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FD97DD5-FFE4-104C-A160-68767F346FE1}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_3A09A587BADDE2F2EEC00F81A82FAC824A35A5A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3E8DAE8-A452-C64B-AA91-48CECEFED39B}"/>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="500" windowWidth="20400" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8400" yWindow="500" windowWidth="20400" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="pcr_known" sheetId="1" r:id="rId1"/>
-    <sheet name="pcr_unknown_rs0.8" sheetId="2" r:id="rId2"/>
-    <sheet name="pcr_unknown_rs0.85" sheetId="3" r:id="rId3"/>
-    <sheet name="pcr_unknown_rs0.9" sheetId="4" r:id="rId4"/>
-    <sheet name="pcr_unknown_rs0.95" sheetId="5" r:id="rId5"/>
-    <sheet name="pcr_unknown_mss3" sheetId="6" r:id="rId6"/>
+    <sheet name="Read me" sheetId="7" r:id="rId1"/>
+    <sheet name="(1) pcr_known" sheetId="1" r:id="rId2"/>
+    <sheet name="(2) pcr_unknown_rs0.8" sheetId="2" r:id="rId3"/>
+    <sheet name="(3) pcr_unknown_rs0.85" sheetId="3" r:id="rId4"/>
+    <sheet name="(4) pcr_unknown_rs0.9" sheetId="4" r:id="rId5"/>
+    <sheet name="(5) pcr_unknown_rs0.95" sheetId="5" r:id="rId6"/>
+    <sheet name="(6) pcr_unknown_mss3" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="616">
   <si>
     <t>ord</t>
   </si>
@@ -1925,6 +1926,770 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83422CE3-8444-B042-8C9C-8DC1A2A734D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8115300" cy="2844800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Binary predictions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> of unobserved ('unknown') hosts for the host exposure model trained on PCR data, based on different optimal thresholding methods.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(1) pcr_known</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> The list of observed ('known') host genera based on PCR data.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(2) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pcr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>_unknown_rs0.8: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The list of unobserved ('unknown') predicted host genera when applying an 80% sensitivity threshold.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(3) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pcr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>_unknown_rs0.85:  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The list of unobserved ('unknown') predicted host genera when applying an 85% sensitivity threshold.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(4) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pcr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>_unknown_rs0.9: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The list of unobserved ('unknown') predicted host genera when applying an 90% sensitivity threshold.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(5) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pcr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>_unknown_rs0.95: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The list of unobserved ('unknown') predicted host genera when applying an 95% sensitivity threshold.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(6)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pcr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>_unknown_mss3:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> The list of unobserved ('unknown') predicted host genera when applying a threshold that maximizes the sum of sensitivity and specificity, otherwise known as the Youden Index.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2205,6 +2970,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578C2E50-8F40-5C49-B2D1-651E0E2E8CA7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
@@ -2869,17 +3647,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G59"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G59" sqref="E2:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2890,7 +3668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2900,17 +3678,8 @@
       <c r="C2" t="s">
         <v>99</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2920,17 +3689,8 @@
       <c r="C3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2940,17 +3700,8 @@
       <c r="C4" t="s">
         <v>101</v>
       </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2960,17 +3711,8 @@
       <c r="C5" t="s">
         <v>102</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2980,17 +3722,8 @@
       <c r="C6" t="s">
         <v>103</v>
       </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3000,17 +3733,8 @@
       <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3020,17 +3744,8 @@
       <c r="C8" t="s">
         <v>105</v>
       </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3040,17 +3755,8 @@
       <c r="C9" t="s">
         <v>106</v>
       </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3060,17 +3766,8 @@
       <c r="C10" t="s">
         <v>107</v>
       </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3080,17 +3777,8 @@
       <c r="C11" t="s">
         <v>108</v>
       </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3100,17 +3788,8 @@
       <c r="C12" t="s">
         <v>110</v>
       </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3120,17 +3799,8 @@
       <c r="C13" t="s">
         <v>112</v>
       </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3140,17 +3810,8 @@
       <c r="C14" t="s">
         <v>113</v>
       </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3160,17 +3821,8 @@
       <c r="C15" t="s">
         <v>115</v>
       </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -3180,17 +3832,8 @@
       <c r="C16" t="s">
         <v>116</v>
       </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -3200,17 +3843,8 @@
       <c r="C17" t="s">
         <v>117</v>
       </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -3220,17 +3854,8 @@
       <c r="C18" t="s">
         <v>119</v>
       </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3240,17 +3865,8 @@
       <c r="C19" t="s">
         <v>121</v>
       </c>
-      <c r="E19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -3260,17 +3876,8 @@
       <c r="C20" t="s">
         <v>122</v>
       </c>
-      <c r="E20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3280,17 +3887,8 @@
       <c r="C21" t="s">
         <v>123</v>
       </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3300,17 +3898,8 @@
       <c r="C22" t="s">
         <v>124</v>
       </c>
-      <c r="E22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3320,17 +3909,8 @@
       <c r="C23" t="s">
         <v>125</v>
       </c>
-      <c r="E23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3340,17 +3920,8 @@
       <c r="C24" t="s">
         <v>126</v>
       </c>
-      <c r="E24" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3360,17 +3931,8 @@
       <c r="C25" t="s">
         <v>127</v>
       </c>
-      <c r="E25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -3380,17 +3942,8 @@
       <c r="C26" t="s">
         <v>128</v>
       </c>
-      <c r="E26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -3400,17 +3953,8 @@
       <c r="C27" t="s">
         <v>129</v>
       </c>
-      <c r="E27" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" t="s">
-        <v>41</v>
-      </c>
-      <c r="G27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -3420,17 +3964,8 @@
       <c r="C28" t="s">
         <v>130</v>
       </c>
-      <c r="E28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -3440,17 +3975,8 @@
       <c r="C29" t="s">
         <v>131</v>
       </c>
-      <c r="E29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -3460,17 +3986,8 @@
       <c r="C30" t="s">
         <v>133</v>
       </c>
-      <c r="E30" t="s">
-        <v>49</v>
-      </c>
-      <c r="F30" t="s">
-        <v>50</v>
-      </c>
-      <c r="G30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -3480,17 +3997,8 @@
       <c r="C31" t="s">
         <v>134</v>
       </c>
-      <c r="E31" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -3500,17 +4008,8 @@
       <c r="C32" t="s">
         <v>136</v>
       </c>
-      <c r="E32" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -3520,17 +4019,8 @@
       <c r="C33" t="s">
         <v>137</v>
       </c>
-      <c r="E33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -3540,17 +4030,8 @@
       <c r="C34" t="s">
         <v>138</v>
       </c>
-      <c r="E34" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -3560,17 +4041,8 @@
       <c r="C35" t="s">
         <v>139</v>
       </c>
-      <c r="E35" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" t="s">
-        <v>60</v>
-      </c>
-      <c r="G35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -3580,17 +4052,8 @@
       <c r="C36" t="s">
         <v>140</v>
       </c>
-      <c r="E36" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -3600,17 +4063,8 @@
       <c r="C37" t="s">
         <v>141</v>
       </c>
-      <c r="E37" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" t="s">
-        <v>63</v>
-      </c>
-      <c r="G37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -3620,17 +4074,8 @@
       <c r="C38" t="s">
         <v>142</v>
       </c>
-      <c r="E38" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" t="s">
-        <v>66</v>
-      </c>
-      <c r="G38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -3640,17 +4085,8 @@
       <c r="C39" t="s">
         <v>144</v>
       </c>
-      <c r="E39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -3660,17 +4096,8 @@
       <c r="C40" t="s">
         <v>145</v>
       </c>
-      <c r="E40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" t="s">
-        <v>66</v>
-      </c>
-      <c r="G40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -3680,17 +4107,8 @@
       <c r="C41" t="s">
         <v>146</v>
       </c>
-      <c r="E41" t="s">
-        <v>57</v>
-      </c>
-      <c r="F41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -3700,17 +4118,8 @@
       <c r="C42" t="s">
         <v>147</v>
       </c>
-      <c r="E42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" t="s">
-        <v>70</v>
-      </c>
-      <c r="G42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>
@@ -3720,17 +4129,8 @@
       <c r="C43" t="s">
         <v>150</v>
       </c>
-      <c r="E43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" t="s">
-        <v>73</v>
-      </c>
-      <c r="G43" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -3740,17 +4140,8 @@
       <c r="C44" t="s">
         <v>151</v>
       </c>
-      <c r="E44" t="s">
-        <v>75</v>
-      </c>
-      <c r="F44" t="s">
-        <v>76</v>
-      </c>
-      <c r="G44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -3760,17 +4151,8 @@
       <c r="C45" t="s">
         <v>152</v>
       </c>
-      <c r="E45" t="s">
-        <v>75</v>
-      </c>
-      <c r="F45" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -3780,17 +4162,8 @@
       <c r="C46" t="s">
         <v>153</v>
       </c>
-      <c r="E46" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" t="s">
-        <v>80</v>
-      </c>
-      <c r="G46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -3800,17 +4173,8 @@
       <c r="C47" t="s">
         <v>154</v>
       </c>
-      <c r="E47" t="s">
-        <v>79</v>
-      </c>
-      <c r="F47" t="s">
-        <v>82</v>
-      </c>
-      <c r="G47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -3820,17 +4184,8 @@
       <c r="C48" t="s">
         <v>155</v>
       </c>
-      <c r="E48" t="s">
-        <v>79</v>
-      </c>
-      <c r="F48" t="s">
-        <v>82</v>
-      </c>
-      <c r="G48" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -3840,17 +4195,8 @@
       <c r="C49" t="s">
         <v>156</v>
       </c>
-      <c r="E49" t="s">
-        <v>79</v>
-      </c>
-      <c r="F49" t="s">
-        <v>82</v>
-      </c>
-      <c r="G49" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -3860,17 +4206,8 @@
       <c r="C50" t="s">
         <v>157</v>
       </c>
-      <c r="E50" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" t="s">
-        <v>82</v>
-      </c>
-      <c r="G50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -3880,17 +4217,8 @@
       <c r="C51" t="s">
         <v>158</v>
       </c>
-      <c r="E51" t="s">
-        <v>79</v>
-      </c>
-      <c r="F51" t="s">
-        <v>87</v>
-      </c>
-      <c r="G51" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -3900,17 +4228,8 @@
       <c r="C52" t="s">
         <v>159</v>
       </c>
-      <c r="E52" t="s">
-        <v>79</v>
-      </c>
-      <c r="F52" t="s">
-        <v>87</v>
-      </c>
-      <c r="G52" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -3920,17 +4239,8 @@
       <c r="C53" t="s">
         <v>160</v>
       </c>
-      <c r="E53" t="s">
-        <v>79</v>
-      </c>
-      <c r="F53" t="s">
-        <v>87</v>
-      </c>
-      <c r="G53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -3940,17 +4250,8 @@
       <c r="C54" t="s">
         <v>162</v>
       </c>
-      <c r="E54" t="s">
-        <v>79</v>
-      </c>
-      <c r="F54" t="s">
-        <v>87</v>
-      </c>
-      <c r="G54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -3960,17 +4261,8 @@
       <c r="C55" t="s">
         <v>163</v>
       </c>
-      <c r="E55" t="s">
-        <v>79</v>
-      </c>
-      <c r="F55" t="s">
-        <v>87</v>
-      </c>
-      <c r="G55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -3980,17 +4272,8 @@
       <c r="C56" t="s">
         <v>164</v>
       </c>
-      <c r="E56" t="s">
-        <v>79</v>
-      </c>
-      <c r="F56" t="s">
-        <v>93</v>
-      </c>
-      <c r="G56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -4000,17 +4283,8 @@
       <c r="C57" t="s">
         <v>165</v>
       </c>
-      <c r="E57" t="s">
-        <v>79</v>
-      </c>
-      <c r="F57" t="s">
-        <v>95</v>
-      </c>
-      <c r="G57" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -4020,17 +4294,8 @@
       <c r="C58" t="s">
         <v>166</v>
       </c>
-      <c r="E58" t="s">
-        <v>79</v>
-      </c>
-      <c r="F58" t="s">
-        <v>95</v>
-      </c>
-      <c r="G58" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -4040,17 +4305,8 @@
       <c r="C59" t="s">
         <v>168</v>
       </c>
-      <c r="E59" t="s">
-        <v>79</v>
-      </c>
-      <c r="F59" t="s">
-        <v>95</v>
-      </c>
-      <c r="G59" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -4061,7 +4317,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -4072,7 +4328,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -4083,7 +4339,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -4094,7 +4350,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -4177,7 +4433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C82"/>
   <sheetViews>
@@ -5093,7 +5349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C211"/>
   <sheetViews>
@@ -7428,7 +7684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C465"/>
   <sheetViews>
@@ -12557,7 +12813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>

</xml_diff>